<commit_message>
finished formatting of T1-T3
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T1.xlsx
+++ b/Outputs/Tables/T1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Variable: Subcategory</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">7 (12%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*All values displayed as mean ± SD for ratio continuous variables or n (%) for dichotomous categorical variables. Percentages for the variant columns were calculated in respect to total patients within a variant (i.e., within column), and percentages for the total column was calculated in respect to the population total.</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -137,16 +140,27 @@
       <name val="Times New Roman"/>
       <i/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <i/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -154,15 +168,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -171,6 +198,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,134 +506,146 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="9" ht="45" customHeight="1">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A9:E9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed footnote table symbols from symbol to letters
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T1.xlsx
+++ b/Outputs/Tables/T1.xlsx
@@ -17,16 +17,16 @@
     <t xml:space="preserve">Variable: Subcategory</t>
   </si>
   <si>
-    <t xml:space="preserve">Follicular*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FV-PTC*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Papillary*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total*</t>
+    <t xml:space="preserve">Follicularᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FV-PTCᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papillaryᵃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalᵃ</t>
   </si>
   <si>
     <t xml:space="preserve">Mean Age (Years)</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">7 (12%)</t>
   </si>
   <si>
-    <t xml:space="preserve">*All values displayed as mean ± SD for ratio continuous variables or n (%) for dichotomous categorical variables. Percentages for the variant columns were calculated in respect to total patients within a variant (i.e., within column), and percentages for the total column was calculated in respect to the population total.</t>
+    <t xml:space="preserve">ᵃ All values displayed as mean ± SD for ratio continuous variables or n (%) for dichotomous categorical variables. Percentages for the variant columns were calculated in respect to total patients within a variant (i.e., within column), and percentages for the total column was calculated in respect to the population total.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
finished correcting ST and supplemental · issue
</commit_message>
<xml_diff>
--- a/Outputs/Tables/T1.xlsx
+++ b/Outputs/Tables/T1.xlsx
@@ -32,16 +32,16 @@
     <t xml:space="preserve">Mean Age (Years)</t>
   </si>
   <si>
-    <t xml:space="preserve">61·1 ± 12·7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59·8 ± 11·2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60·6 ± 11·5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60·5 ± 11·6</t>
+    <t xml:space="preserve">61.1 ± 12.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.8 ± 11.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.6 ± 11.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.5 ± 11.6</t>
   </si>
   <si>
     <t xml:space="preserve">Sex (Female)</t>

</xml_diff>